<commit_message>
Adding progress reports for Batch and Webpage sprints (incomplete).
</commit_message>
<xml_diff>
--- a/deliverables/Burn-Down.xlsx
+++ b/deliverables/Burn-Down.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="24915" windowHeight="12075"/>
+    <workbookView xWindow="120" yWindow="120" windowWidth="24240" windowHeight="12075"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Sprint</t>
   </si>
@@ -45,17 +45,26 @@
     <t>Delta</t>
   </si>
   <si>
-    <t>Story Points</t>
-  </si>
-  <si>
     <t>Predicted Story Points Remaining</t>
+  </si>
+  <si>
+    <t>Total:</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Planned Story Points</t>
+  </si>
+  <si>
+    <t>Actual Story Points</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -92,7 +101,263 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-CA"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Predicted Story Points Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Prototype</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Profiling</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Docs and Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$E$2:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual Story Points Remaining</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Prototype</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Webpage</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Batch</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Profiling</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Completion</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Docs and Demo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$2:$F$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="44434560"/>
+        <c:axId val="44436096"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="44434560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44436096"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="44436096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="44434560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -170,6 +435,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -204,6 +470,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -379,39 +646,47 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="31.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -419,18 +694,24 @@
         <v>29.5</v>
       </c>
       <c r="C2">
+        <v>29.5</v>
+      </c>
+      <c r="D2">
+        <v>29.5</v>
+      </c>
+      <c r="E2">
         <f>SUM(B3:B7)</f>
         <v>141</v>
       </c>
-      <c r="D2">
-        <v>141</v>
-      </c>
-      <c r="E2">
-        <f>C2-D2</f>
-        <v>0</v>
+      <c r="F2">
+        <v>144</v>
+      </c>
+      <c r="G2">
+        <f>E2-F2</f>
+        <v>-3</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -438,15 +719,25 @@
         <v>33</v>
       </c>
       <c r="C3">
+        <v>36</v>
+      </c>
+      <c r="D3">
+        <v>26</v>
+      </c>
+      <c r="E3">
         <f>SUM(B4:B7)</f>
         <v>108</v>
       </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E7" si="0">C3-D3</f>
-        <v>108</v>
+      <c r="F3">
+        <f>SUM(B2:B7)-SUM(D2:D3)</f>
+        <v>115</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G7" si="0">E3-F3</f>
+        <v>-7</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -454,85 +745,98 @@
         <v>33</v>
       </c>
       <c r="C4">
+        <v>43</v>
+      </c>
+      <c r="E4">
         <f>SUM(B5:B7)</f>
         <v>75</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5">
         <v>37</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <f>SUM(B6:B7)</f>
         <v>38</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
       <c r="B6">
         <v>29.5</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <f>SUM(B7)</f>
         <v>8.5</v>
       </c>
-      <c r="E6">
+      <c r="G6">
         <f t="shared" si="0"/>
         <v>8.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <v>8.5</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="E7">
+      <c r="G7">
         <f t="shared" si="0"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <f>SUM(B2:B7)</f>
+        <v>170.5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>